<commit_message>
added a retry function. Last night the noun phrase of IBB failed to complete. Now the the application will check the outpu box to ensure that all have completed. On a side note I have fixed the issue of the results appearing at a seperate time. I did this using Task.AwaitAll()
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/Trades/BIIB/BIIBBagTrade.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/Trades/BIIB/BIIBBagTrade.xlsx
@@ -366,7 +366,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -568,6 +568,32 @@
         <v>1</v>
       </c>
     </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9758.1299999999992</v>
+      </c>
+      <c r="B9">
+        <v>9815.06</v>
+      </c>
+      <c r="C9">
+        <v>307.20999999999998</v>
+      </c>
+      <c r="D9">
+        <v>305.42</v>
+      </c>
+      <c r="E9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>-0.57999999999999996</v>
+      </c>
+      <c r="G9" s="1">
+        <v>42609.488958333335</v>
+      </c>
+      <c r="H9" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added a method to retrieve the fundamentals from the stock
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/Trades/BIIB/BIIBBagTrade.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/Trades/BIIB/BIIBBagTrade.xlsx
@@ -366,7 +366,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -776,6 +776,32 @@
         <v>0</v>
       </c>
     </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>9300.5300000000007</v>
+      </c>
+      <c r="B17">
+        <v>9578.2999999999993</v>
+      </c>
+      <c r="C17">
+        <v>294.14</v>
+      </c>
+      <c r="D17">
+        <v>302.66000000000003</v>
+      </c>
+      <c r="E17" t="b">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>2.9</v>
+      </c>
+      <c r="G17" s="1">
+        <v>42626.544317129628</v>
+      </c>
+      <c r="H17" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
traded noticed a bug
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/Trades/BIIB/BIIBBagTrade.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/Trades/BIIB/BIIBBagTrade.xlsx
@@ -369,7 +369,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -448,6 +448,35 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>42635.642870370371</v>
+      </c>
+      <c r="B4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>9951.5</v>
+      </c>
+      <c r="D4">
+        <v>10000</v>
+      </c>
+      <c r="E4">
+        <v>309</v>
+      </c>
+      <c r="F4">
+        <v>312</v>
+      </c>
+      <c r="G4" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>0.97</v>
+      </c>
+      <c r="I4" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
trades. Fixed a bug with the trading module.
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/Trades/BIIB/BIIBBagTrade.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/Trades/BIIB/BIIBBagTrade.xlsx
@@ -369,7 +369,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -477,6 +477,35 @@
         <v>0</v>
       </c>
     </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>42636.593078703707</v>
+      </c>
+      <c r="B5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>9979.36</v>
+      </c>
+      <c r="D5">
+        <v>9951.5</v>
+      </c>
+      <c r="E5">
+        <v>313.07</v>
+      </c>
+      <c r="F5">
+        <v>314.81</v>
+      </c>
+      <c r="G5" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="I5" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>